<commit_message>
Login with different valid and invalid logins
</commit_message>
<xml_diff>
--- a/Framework/testdata/OrangeHRM-TestData.xlsx
+++ b/Framework/testdata/OrangeHRM-TestData.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\selenium-apr-2016\Peter\OrangeHRM\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="11310" windowHeight="480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="AuthTests" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Column1</t>
   </si>
@@ -67,17 +63,17 @@
     <t>invalid</t>
   </si>
   <si>
-    <t>longvalidusername</t>
-  </si>
-  <si>
-    <t>longvalidpassword</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,7 +250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,40 +427,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:E33"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:9">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -487,13 +483,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9">
       <c r="E7" s="1"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9">
       <c r="F9" s="1"/>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9">
       <c r="C16" t="s">
         <v>0</v>
       </c>
@@ -516,7 +512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5">
       <c r="C24" t="s">
         <v>7</v>
       </c>
@@ -527,18 +523,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:5">
       <c r="C25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5">
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -549,15 +545,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:5">
       <c r="C27" t="s">
         <v>10</v>
       </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:5">
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
@@ -565,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:5">
       <c r="C29" t="s">
         <v>12</v>
       </c>
@@ -576,12 +578,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:5">
       <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
         <v>13</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -598,12 +600,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Employee data drive test is added
</commit_message>
<xml_diff>
--- a/Framework/testdata/OrangeHRM-TestData.xlsx
+++ b/Framework/testdata/OrangeHRM-TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="11310" windowHeight="480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13245" windowHeight="5355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -22,28 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -67,6 +46,60 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>NameA</t>
+  </si>
+  <si>
+    <t>NameB</t>
+  </si>
+  <si>
+    <t>NameC</t>
+  </si>
+  <si>
+    <t>NameD</t>
+  </si>
+  <si>
+    <t>NameE</t>
+  </si>
+  <si>
+    <t>Middle1</t>
+  </si>
+  <si>
+    <t>Middle2</t>
+  </si>
+  <si>
+    <t>Middle3</t>
+  </si>
+  <si>
+    <t>Middle4</t>
+  </si>
+  <si>
+    <t>Middle5</t>
+  </si>
+  <si>
+    <t>Last1</t>
+  </si>
+  <si>
+    <t>Last2</t>
+  </si>
+  <si>
+    <t>Last3</t>
+  </si>
+  <si>
+    <t>Last4</t>
+  </si>
+  <si>
+    <t>Last5</t>
   </si>
 </sst>
 </file>
@@ -82,18 +115,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,9 +135,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,44 +155,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="addEmployeeTestData" displayName="addEmployeeTestData" ref="C3:I12" totalsRowShown="0">
-  <autoFilter ref="C3:I12"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="loginTestData" displayName="loginTestData" ref="C16:I22" totalsRowShown="0">
-  <autoFilter ref="C16:I22"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RightLoginTestData" displayName="RightLoginTestData" ref="C24:E30" totalsRowShown="0">
   <autoFilter ref="C24:E30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Username"/>
     <tableColumn id="2" name="Password"/>
     <tableColumn id="3" name="Expected"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="EmployeeDetails" displayName="EmployeeDetails" ref="D3:F8" totalsRowShown="0">
+  <autoFilter ref="D3:F8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="FirstName"/>
+    <tableColumn id="2" name="MiddleName"/>
+    <tableColumn id="3" name="LastName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,88 +453,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:I30"/>
+  <dimension ref="C3:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
+    <row r="3" spans="4:6">
       <c r="D3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="9" spans="3:9">
-      <c r="F9" s="1"/>
-    </row>
-    <row r="16" spans="3:9">
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="3:5">
       <c r="C24" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="3:5">
       <c r="C25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -536,10 +558,10 @@
     </row>
     <row r="26" spans="3:5">
       <c r="C26" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -547,10 +569,10 @@
     </row>
     <row r="27" spans="3:5">
       <c r="C27" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -558,10 +580,10 @@
     </row>
     <row r="28" spans="3:5">
       <c r="C28" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -569,10 +591,10 @@
     </row>
     <row r="29" spans="3:5">
       <c r="C29" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -580,10 +602,10 @@
     </row>
     <row r="30" spans="3:5">
       <c r="C30" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -591,8 +613,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>

</xml_diff>